<commit_message>
add conditions and some more analysis
</commit_message>
<xml_diff>
--- a/Analysis/sheet.xlsx
+++ b/Analysis/sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51968B0-A82B-4FF2-845F-5E8D6B82D6AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF41D6D4-0EE4-4609-B144-16E430542170}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,17 +11,23 @@
     <sheet name="Test 1" sheetId="1" r:id="rId1"/>
     <sheet name="Test 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
   <si>
     <t>#</t>
   </si>
@@ -126,12 +132,6 @@
   </si>
   <si>
     <t>o3</t>
-  </si>
-  <si>
-    <t>p4</t>
-  </si>
-  <si>
-    <t>o4</t>
   </si>
 </sst>
 </file>
@@ -247,6 +247,25 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -270,25 +289,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -359,13 +359,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3B4F013B-6174-440D-901B-CCCB736FD0BD}" name="Table3" displayName="Table3" ref="O2:R5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3B4F013B-6174-440D-901B-CCCB736FD0BD}" name="Table3" displayName="Table3" ref="O2:R5" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="O2:R5" xr:uid="{AFF03743-4729-4AE0-A300-5E7F4FF83E2C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AA94CBAC-BCC8-4523-BD98-7075C3946061}" name="Orden" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{084F57AE-7823-4D58-B39C-30B0BC0807D0}" name="Hours" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{352BEC57-A4F1-4C0F-B925-BA7DD498ED26}" name="Setup" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{5DFBDDDE-47D4-4CD3-A109-D78758180307}" name="Piezas por hacer" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{AA94CBAC-BCC8-4523-BD98-7075C3946061}" name="Orden" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{084F57AE-7823-4D58-B39C-30B0BC0807D0}" name="Hours" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{352BEC57-A4F1-4C0F-B925-BA7DD498ED26}" name="Setup" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{5DFBDDDE-47D4-4CD3-A109-D78758180307}" name="Piezas por hacer" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -401,13 +401,13 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DF5248E3-CD80-4D61-9BF6-9EC928199AE6}" name="Table6" displayName="Table6" ref="N1:Q5" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DF5248E3-CD80-4D61-9BF6-9EC928199AE6}" name="Table6" displayName="Table6" ref="N1:Q5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="N1:Q5" xr:uid="{143F0776-70FE-4706-87F9-EDF727246CEA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4D1EA108-50FC-4591-A45D-133B4361787B}" name="Orden" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{7FDAFE89-7255-425A-B95A-3D355A2DF70B}" name="Hours" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{28F5E592-9C6F-4ACC-BFAE-2EAFEFA9E226}" name="Setup" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{3A09B1F3-29EB-4616-B133-89F4BC4E1414}" name="Piezas por hacer" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{4D1EA108-50FC-4591-A45D-133B4361787B}" name="Orden" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{7FDAFE89-7255-425A-B95A-3D355A2DF70B}" name="Hours" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{28F5E592-9C6F-4ACC-BFAE-2EAFEFA9E226}" name="Setup" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{3A09B1F3-29EB-4616-B133-89F4BC4E1414}" name="Piezas por hacer" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -950,7 +950,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,6 +1031,9 @@
       <c r="E2">
         <v>1.2</v>
       </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
       <c r="K2" t="s">
         <v>16</v>
       </c>
@@ -1066,6 +1069,9 @@
       <c r="E3">
         <v>0.4</v>
       </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
       <c r="K3" t="s">
         <v>17</v>
       </c>
@@ -1087,7 +1093,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
@@ -1096,10 +1102,13 @@
         <v>34</v>
       </c>
       <c r="D4">
-        <v>5.4</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0.8</v>
+        <v>0.4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
       </c>
       <c r="K4" t="s">
         <v>18</v>
@@ -1125,16 +1134,19 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>5.4</v>
       </c>
       <c r="E5">
-        <v>1.9</v>
+        <v>0.4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
       </c>
       <c r="N5" s="9">
         <v>4</v>
@@ -1150,21 +1162,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6">
-        <v>6.8</v>
-      </c>
-      <c r="E6">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>

</xml_diff>

<commit_message>
fix test involving days
</commit_message>
<xml_diff>
--- a/Analysis/sheet.xlsx
+++ b/Analysis/sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Test 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="43">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t xml:space="preserve">COMENTARIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEDNESDAY</t>
   </si>
   <si>
     <t xml:space="preserve">Test</t>
@@ -1508,8 +1511,8 @@
   </sheetPr>
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3225,8 +3228,8 @@
   </sheetPr>
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3305,6 +3308,9 @@
       <c r="D2" s="8" t="n">
         <v>7.2</v>
       </c>
+      <c r="H2" s="0" t="s">
+        <v>17</v>
+      </c>
       <c r="J2" s="0" t="s">
         <v>18</v>
       </c>
@@ -3333,6 +3339,9 @@
       </c>
       <c r="C3" s="8" t="n">
         <v>8.1</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>20</v>
@@ -3355,6 +3364,9 @@
       <c r="C4" s="8" t="n">
         <v>5.5</v>
       </c>
+      <c r="H4" s="0" t="s">
+        <v>17</v>
+      </c>
       <c r="J4" s="0" t="s">
         <v>22</v>
       </c>
@@ -3376,6 +3388,9 @@
       <c r="C5" s="8" t="n">
         <v>8.5</v>
       </c>
+      <c r="H5" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
@@ -3391,6 +3406,9 @@
       <c r="C6" s="8" t="n">
         <v>8.1</v>
       </c>
+      <c r="H6" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
@@ -3402,6 +3420,9 @@
       <c r="C7" s="8" t="n">
         <v>5.5</v>
       </c>
+      <c r="H7" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
@@ -3413,6 +3434,9 @@
       <c r="C8" s="8" t="n">
         <v>8.5</v>
       </c>
+      <c r="H8" s="0" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
@@ -3424,13 +3448,16 @@
       <c r="C9" s="8" t="n">
         <v>7.5</v>
       </c>
+      <c r="H9" s="0" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>